<commit_message>
Fixes and now inlcuding interactive sankey page
</commit_message>
<xml_diff>
--- a/ass_3/3/fix1_community_switching_detailed.xlsx
+++ b/ass_3/3/fix1_community_switching_detailed.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="35">
   <si>
     <t>Community</t>
   </si>
@@ -117,7 +117,22 @@
     <t>-&gt; 2010</t>
   </si>
   <si>
-    <t>-&gt; 2011</t>
+    <t>DB (0)</t>
+  </si>
+  <si>
+    <t>AL &amp; ML (1)</t>
+  </si>
+  <si>
+    <t>IR (2)</t>
+  </si>
+  <si>
+    <t>DM (3)</t>
+  </si>
+  <si>
+    <t>AL &amp; TH (4)</t>
+  </si>
+  <si>
+    <t>CV (5)</t>
   </si>
 </sst>
 </file>
@@ -187,26 +202,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Microsoft Sans Serif"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="26">
     <dxf>
       <font>
         <b val="0"/>
@@ -689,46 +685,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel2" displayName="Tabel2" ref="A1:L37" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
-  <autoFilter ref="A1:L37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel2" displayName="Tabel2" ref="A1:K37" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="A1:K37"/>
   <sortState ref="A2:K37">
     <sortCondition ref="B1:B37"/>
   </sortState>
-  <tableColumns count="12">
-    <tableColumn id="1" name="Community" dataDxfId="24"/>
-    <tableColumn id="2" name="Type" dataDxfId="23"/>
-    <tableColumn id="3" name="2001 -&gt; 2002" dataDxfId="22"/>
-    <tableColumn id="4" name="-&gt; 2003" dataDxfId="21"/>
-    <tableColumn id="5" name=" -&gt; 2004" dataDxfId="20"/>
-    <tableColumn id="6" name="-&gt; 2005" dataDxfId="19"/>
-    <tableColumn id="7" name="-&gt; 2006" dataDxfId="18"/>
-    <tableColumn id="8" name="-&gt; 2007" dataDxfId="17"/>
-    <tableColumn id="9" name="-&gt; 2008" dataDxfId="16"/>
-    <tableColumn id="10" name="-&gt; 2009" dataDxfId="15"/>
-    <tableColumn id="11" name="-&gt; 2010" dataDxfId="14"/>
-    <tableColumn id="12" name="-&gt; 2011" dataDxfId="0">
-      <calculatedColumnFormula>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</calculatedColumnFormula>
-    </tableColumn>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Community" dataDxfId="23"/>
+    <tableColumn id="2" name="Type" dataDxfId="22"/>
+    <tableColumn id="3" name="2001 -&gt; 2002" dataDxfId="21"/>
+    <tableColumn id="4" name="-&gt; 2003" dataDxfId="20"/>
+    <tableColumn id="5" name=" -&gt; 2004" dataDxfId="19"/>
+    <tableColumn id="6" name="-&gt; 2005" dataDxfId="18"/>
+    <tableColumn id="7" name="-&gt; 2006" dataDxfId="17"/>
+    <tableColumn id="8" name="-&gt; 2007" dataDxfId="16"/>
+    <tableColumn id="9" name="-&gt; 2008" dataDxfId="15"/>
+    <tableColumn id="10" name="-&gt; 2009" dataDxfId="14"/>
+    <tableColumn id="11" name="-&gt; 2010" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:K31" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:K31" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:K31"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="Community" dataDxfId="11"/>
-    <tableColumn id="2" name="Type" dataDxfId="10"/>
-    <tableColumn id="3" name="2001 -&gt; 2002" dataDxfId="9"/>
-    <tableColumn id="4" name="2002 -&gt; 2003" dataDxfId="8"/>
-    <tableColumn id="5" name="2003 -&gt; 2004" dataDxfId="7"/>
-    <tableColumn id="6" name="2004 -&gt; 2005" dataDxfId="6"/>
-    <tableColumn id="7" name="2005 -&gt; 2006" dataDxfId="5"/>
-    <tableColumn id="8" name="2006 -&gt; 2007" dataDxfId="4"/>
-    <tableColumn id="9" name="2007 -&gt; 2008" dataDxfId="3"/>
-    <tableColumn id="10" name="2008 -&gt; 2009" dataDxfId="2"/>
-    <tableColumn id="11" name="2009 -&gt; 2010" dataDxfId="1"/>
+    <tableColumn id="1" name="Community" dataDxfId="10"/>
+    <tableColumn id="2" name="Type" dataDxfId="9"/>
+    <tableColumn id="3" name="2001 -&gt; 2002" dataDxfId="8"/>
+    <tableColumn id="4" name="2002 -&gt; 2003" dataDxfId="7"/>
+    <tableColumn id="5" name="2003 -&gt; 2004" dataDxfId="6"/>
+    <tableColumn id="6" name="2004 -&gt; 2005" dataDxfId="5"/>
+    <tableColumn id="7" name="2005 -&gt; 2006" dataDxfId="4"/>
+    <tableColumn id="8" name="2006 -&gt; 2007" dataDxfId="3"/>
+    <tableColumn id="9" name="2007 -&gt; 2008" dataDxfId="2"/>
+    <tableColumn id="10" name="2008 -&gt; 2009" dataDxfId="1"/>
+    <tableColumn id="11" name="2009 -&gt; 2010" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1000,10 +993,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1015,7 +1008,7 @@
     <col min="12" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1049,13 +1042,10 @@
       <c r="K1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>15</v>
@@ -1087,14 +1077,10 @@
       <c r="K2" s="1">
         <v>259</v>
       </c>
-      <c r="L2" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>3143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
@@ -1126,14 +1112,10 @@
       <c r="K3" s="1">
         <v>442</v>
       </c>
-      <c r="L3" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>5673</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>15</v>
@@ -1165,14 +1147,10 @@
       <c r="K4" s="1">
         <v>263</v>
       </c>
-      <c r="L4" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>2140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>3</v>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>15</v>
@@ -1204,14 +1182,10 @@
       <c r="K5" s="1">
         <v>452</v>
       </c>
-      <c r="L5" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>4224</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>4</v>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>15</v>
@@ -1243,14 +1217,10 @@
       <c r="K6" s="1">
         <v>235</v>
       </c>
-      <c r="L6" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>2312</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>5</v>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>15</v>
@@ -1282,14 +1252,10 @@
       <c r="K7" s="1">
         <v>594</v>
       </c>
-      <c r="L7" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>4649</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>0</v>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
@@ -1321,14 +1287,10 @@
       <c r="K8" s="1">
         <v>556</v>
       </c>
-      <c r="L8" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>4258</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>1</v>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>11</v>
@@ -1360,14 +1322,10 @@
       <c r="K9" s="1">
         <v>794</v>
       </c>
-      <c r="L9" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>7152</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>2</v>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>11</v>
@@ -1399,14 +1357,10 @@
       <c r="K10" s="1">
         <v>401</v>
       </c>
-      <c r="L10" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>2532</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>3</v>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
@@ -1438,14 +1392,10 @@
       <c r="K11" s="1">
         <v>869</v>
       </c>
-      <c r="L11" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>5035</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>4</v>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>11</v>
@@ -1477,14 +1427,10 @@
       <c r="K12" s="1">
         <v>402</v>
       </c>
-      <c r="L12" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>3160</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>5</v>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>11</v>
@@ -1516,14 +1462,10 @@
       <c r="K13" s="1">
         <v>1196</v>
       </c>
-      <c r="L13" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>5621</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>0</v>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>20</v>
@@ -1555,14 +1497,10 @@
       <c r="K14" s="1">
         <v>187</v>
       </c>
-      <c r="L14" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>1305</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>1</v>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>20</v>
@@ -1594,14 +1532,10 @@
       <c r="K15" s="1">
         <v>335</v>
       </c>
-      <c r="L15" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>2040</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>2</v>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>20</v>
@@ -1633,14 +1567,10 @@
       <c r="K16" s="1">
         <v>136</v>
       </c>
-      <c r="L16" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>766</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>3</v>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>20</v>
@@ -1672,14 +1602,10 @@
       <c r="K17" s="1">
         <v>219</v>
       </c>
-      <c r="L17" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>1417</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>4</v>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>20</v>
@@ -1711,14 +1637,10 @@
       <c r="K18" s="1">
         <v>177</v>
       </c>
-      <c r="L18" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>5</v>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>20</v>
@@ -1750,14 +1672,10 @@
       <c r="K19" s="1">
         <v>271</v>
       </c>
-      <c r="L19" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>1730</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>0</v>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>12</v>
@@ -1789,14 +1707,10 @@
       <c r="K20" s="1">
         <v>146</v>
       </c>
-      <c r="L20" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>1537</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>1</v>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>12</v>
@@ -1828,14 +1742,10 @@
       <c r="K21" s="1">
         <v>194</v>
       </c>
-      <c r="L21" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>1411</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>2</v>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>12</v>
@@ -1867,14 +1777,10 @@
       <c r="K22" s="1">
         <v>73</v>
       </c>
-      <c r="L22" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>426</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>3</v>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>12</v>
@@ -1906,14 +1812,10 @@
       <c r="K23" s="1">
         <v>144</v>
       </c>
-      <c r="L23" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>997</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>4</v>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>12</v>
@@ -1945,14 +1847,10 @@
       <c r="K24" s="1">
         <v>65</v>
       </c>
-      <c r="L24" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>961</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>5</v>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>12</v>
@@ -1984,14 +1882,10 @@
       <c r="K25" s="1">
         <v>362</v>
       </c>
-      <c r="L25" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>1435</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>0</v>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>13</v>
@@ -2023,14 +1917,10 @@
       <c r="K26" s="1">
         <v>128</v>
       </c>
-      <c r="L26" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>1128</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>1</v>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>13</v>
@@ -2062,14 +1952,10 @@
       <c r="K27" s="1">
         <v>359</v>
       </c>
-      <c r="L27" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>1762</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>2</v>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>13</v>
@@ -2101,14 +1987,10 @@
       <c r="K28" s="1">
         <v>131</v>
       </c>
-      <c r="L28" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>850</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>3</v>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>13</v>
@@ -2140,14 +2022,10 @@
       <c r="K29" s="1">
         <v>243</v>
       </c>
-      <c r="L29" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>1890</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>4</v>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>13</v>
@@ -2179,14 +2057,10 @@
       <c r="K30" s="1">
         <v>150</v>
       </c>
-      <c r="L30" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>1040</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>5</v>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>13</v>
@@ -2218,14 +2092,10 @@
       <c r="K31" s="1">
         <v>192</v>
       </c>
-      <c r="L31" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>907</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>0</v>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>14</v>
@@ -2257,14 +2127,10 @@
       <c r="K32" s="1">
         <v>182</v>
       </c>
-      <c r="L32" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>1151</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
-        <v>1</v>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>14</v>
@@ -2296,14 +2162,10 @@
       <c r="K33" s="1">
         <v>225</v>
       </c>
-      <c r="L33" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>1708</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <v>2</v>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>14</v>
@@ -2335,14 +2197,10 @@
       <c r="K34" s="1">
         <v>145</v>
       </c>
-      <c r="L34" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>813</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <v>3</v>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>14</v>
@@ -2374,14 +2232,10 @@
       <c r="K35" s="1">
         <v>304</v>
       </c>
-      <c r="L35" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
-        <v>4</v>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>14</v>
@@ -2413,14 +2267,10 @@
       <c r="K36" s="1">
         <v>147</v>
       </c>
-      <c r="L36" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>1069</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
-        <v>5</v>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>14</v>
@@ -2451,10 +2301,6 @@
       </c>
       <c r="K37" s="1">
         <v>200</v>
-      </c>
-      <c r="L37" s="1">
-        <f>SUM(Tabel2[[#This Row],[2001 -&gt; 2002]:[-&gt; 2010]])</f>
-        <v>826</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new image and small excel changes
</commit_message>
<xml_diff>
--- a/ass_3/3/fix1_community_switching_detailed.xlsx
+++ b/ass_3/3/fix1_community_switching_detailed.xlsx
@@ -996,7 +996,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2327,8 +2327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W132"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>